<commit_message>
Add payment function. COD
</commit_message>
<xml_diff>
--- a/.Bao Cao Group H/CheckList_GroupH.xlsx
+++ b/.Bao Cao Group H/CheckList_GroupH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCHOOL\PROJECT\k12110323\.Bao Cao Group H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCHOOL\PROJECT\GroupBuy\.Bao Cao Group H\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -930,8 +930,8 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1009,13 +1009,13 @@
         <v>18.5</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="44">
+      <c r="H5" s="45">
         <f>SUM(H7:H59)</f>
-        <v>6.4899999999999984</v>
+        <v>7.8999999999999977</v>
       </c>
       <c r="I5" s="44">
         <f>SUM(I7:I59)</f>
-        <v>4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1032,7 +1032,7 @@
       <c r="G6" s="17">
         <v>1</v>
       </c>
-      <c r="H6" s="42"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1389,10 +1389,10 @@
         <v>0.5</v>
       </c>
       <c r="H26" s="46">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I26" s="46">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1410,10 +1410,10 @@
         <v>0.5</v>
       </c>
       <c r="H27" s="46">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I27" s="46">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,7 +1582,9 @@
       <c r="G37" s="19">
         <v>0.18</v>
       </c>
-      <c r="H37" s="45"/>
+      <c r="H37" s="19">
+        <v>0.18</v>
+      </c>
       <c r="I37" s="45"/>
     </row>
     <row r="38" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1599,7 +1601,9 @@
       <c r="G38" s="19">
         <v>0.18</v>
       </c>
-      <c r="H38" s="45"/>
+      <c r="H38" s="19">
+        <v>0.18</v>
+      </c>
       <c r="I38" s="45"/>
     </row>
     <row r="39" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1616,7 +1620,7 @@
       <c r="G39" s="19">
         <v>0.18</v>
       </c>
-      <c r="H39" s="46">
+      <c r="H39" s="19">
         <v>0.18</v>
       </c>
       <c r="I39" s="45"/>
@@ -1635,7 +1639,7 @@
       <c r="G40" s="19">
         <v>0.25</v>
       </c>
-      <c r="H40" s="46">
+      <c r="H40" s="19">
         <v>0.25</v>
       </c>
       <c r="I40" s="45"/>
@@ -1654,7 +1658,7 @@
       <c r="G41" s="19">
         <v>0.18</v>
       </c>
-      <c r="H41" s="46">
+      <c r="H41" s="19">
         <v>0.18</v>
       </c>
       <c r="I41" s="45"/>
@@ -1690,7 +1694,7 @@
       <c r="G43" s="19">
         <v>0.18</v>
       </c>
-      <c r="H43" s="46">
+      <c r="H43" s="19">
         <v>0.18</v>
       </c>
       <c r="I43" s="45"/>
@@ -1726,7 +1730,9 @@
       <c r="G45" s="19">
         <v>0.2</v>
       </c>
-      <c r="H45" s="45"/>
+      <c r="H45" s="19">
+        <v>0.2</v>
+      </c>
       <c r="I45" s="45"/>
     </row>
     <row r="46" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1864,7 +1870,7 @@
       <c r="G53" s="19">
         <v>0.35</v>
       </c>
-      <c r="H53" s="46">
+      <c r="H53" s="19">
         <v>0.35</v>
       </c>
       <c r="I53" s="45"/>
@@ -1883,7 +1889,7 @@
       <c r="G54" s="19">
         <v>0.35</v>
       </c>
-      <c r="H54" s="46">
+      <c r="H54" s="19">
         <v>0.35</v>
       </c>
       <c r="I54" s="45"/>
@@ -1902,7 +1908,9 @@
       <c r="G55" s="19">
         <v>0.35</v>
       </c>
-      <c r="H55" s="45"/>
+      <c r="H55" s="19">
+        <v>0.35</v>
+      </c>
       <c r="I55" s="45"/>
     </row>
     <row r="56" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>